<commit_message>
#56 and fixes #57
</commit_message>
<xml_diff>
--- a/mutualite-rh/chequedej/fr.mutualite.rh.chequedej.model.editor/template/template-saisie.xlsx
+++ b/mutualite-rh/chequedej/fr.mutualite.rh.chequedej.model.editor/template/template-saisie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Saisie" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t> Commande Chèque Dejeuner </t>
   </si>
@@ -40,10 +40,18 @@
     <t>Nombre de jours entiers prévus pour </t>
   </si>
   <si>
+    <t>Si un salarié manque dans la liste, 
+merci de le rajouter manuellement, 
+Même si vous ne connaissez pas le matricule !</t>
+  </si>
+  <si>
     <t>HALLIDAY</t>
   </si>
   <si>
     <t>Johnny</t>
+  </si>
+  <si>
+    <t>Temps complet</t>
   </si>
 </sst>
 </file>
@@ -55,7 +63,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -78,6 +86,12 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="20"/>
       <name val="Arial"/>
@@ -85,6 +99,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="15"/>
       <name val="Arial"/>
@@ -92,7 +112,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b val="true"/>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -109,6 +130,23 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="13"/>
+      <color rgb="FFFF3333"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -168,45 +206,69 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -230,18 +292,22 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <i val="1"/>
+        <color rgb="FFCC3300"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <name val="Arial"/>
         <charset val="1"/>
         <family val="2"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3333"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <colors>
@@ -298,7 +364,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFCC3300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -312,99 +378,104 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="88.9591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="47.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+    <row r="4" customFormat="false" ht="88.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="14" t="s">
         <v>5</v>
       </c>
+      <c r="H4" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1532</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="C5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="n">
+      <c r="F5" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="J5" s="11"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
+      <c r="K5" s="17"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
   </mergeCells>
-  <conditionalFormatting sqref="J5">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND(T($B5)="",T(A5)="")</formula>
+  <conditionalFormatting sqref="D5:D400">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Temps partiel"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:A414">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>T($B5)=="" and T(A5)=""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:E501">
-    <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>AND(NOT(ISBLANK($B5)),ISBLANK(A5))</formula>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Temps complet"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>